<commit_message>
fixed export features and minor changes in FE
</commit_message>
<xml_diff>
--- a/assets.xlsx
+++ b/assets.xlsx
@@ -1,45 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sherabwangchuk/Desktop/ATA/AssetTagging/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E01E6451-129E-044F-94C5-3C91EF887701}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -58,22 +49,81 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -361,64 +411,195 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="G2:G15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="19.83203125" customWidth="1"/>
-    <col min="2" max="2" width="23.5" customWidth="1"/>
-    <col min="3" max="3" width="18.5" customWidth="1"/>
-    <col min="5" max="5" width="24.5" customWidth="1"/>
-    <col min="6" max="6" width="25.6640625" customWidth="1"/>
-    <col min="7" max="7" width="39.5" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="2" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G2" s="1"/>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Asset ID</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Category</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Sub Category</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Location</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Owner</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Purchase Date</t>
+        </is>
+      </c>
     </row>
-    <row r="3" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G3" s="1"/>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>347890</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>scoreboard</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>sports</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>basketball scoreboard</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>SSO office</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>SSO</t>
+        </is>
+      </c>
+      <c r="G2" s="1" t="n">
+        <v>44948</v>
+      </c>
     </row>
-    <row r="4" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G4" s="1"/>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>123456</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>filter</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>dorm_amenities</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>drinking filter</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>h17</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>sherab</t>
+        </is>
+      </c>
+      <c r="G3" s="1" t="n">
+        <v>44898</v>
+      </c>
     </row>
-    <row r="5" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G5" s="1"/>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>1234567</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Table</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>dorm_amenities</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>asdfdsfad</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>h17</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Dorji</t>
+        </is>
+      </c>
+      <c r="G4" s="1" t="n">
+        <v>45282</v>
+      </c>
     </row>
-    <row r="6" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G6" s="1"/>
-    </row>
-    <row r="7" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G7" s="1"/>
-    </row>
-    <row r="8" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G8" s="1"/>
-    </row>
-    <row r="9" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G9" s="1"/>
-    </row>
-    <row r="10" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G10" s="1"/>
-    </row>
-    <row r="11" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G11" s="1"/>
-    </row>
-    <row r="12" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G12" s="1"/>
-    </row>
-    <row r="13" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G13" s="1"/>
-    </row>
-    <row r="14" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G14" s="1"/>
-    </row>
-    <row r="15" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G15" s="1"/>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>7890</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Chair</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>dorm_amenities</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Study chair</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>h17</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Pema</t>
+        </is>
+      </c>
+      <c r="G5" s="1" t="n">
+        <v>45263</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
fixed pagination,modal bugs and added notification
</commit_message>
<xml_diff>
--- a/assets.xlsx
+++ b/assets.xlsx
@@ -416,7 +416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -464,47 +464,47 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>347890</t>
+          <t>4325</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>scoreboard</t>
+          <t>asdf</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>sports</t>
+          <t>dorm_amenities</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>basketball scoreboard</t>
+          <t>asdfdsfad</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>SSO office</t>
+          <t>adasdf</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>SSO</t>
+          <t>asdf</t>
         </is>
       </c>
       <c r="G2" s="1" t="n">
-        <v>44948</v>
+        <v>44898</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>123456</t>
+          <t>432141</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>filter</t>
+          <t>Table</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -514,7 +514,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>drinking filter</t>
+          <t>asdfdsfad</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -524,7 +524,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>sherab</t>
+          <t>Dorji</t>
         </is>
       </c>
       <c r="G3" s="1" t="n">
@@ -534,71 +534,1541 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>1234567</t>
+          <t>9876977</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Table</t>
+          <t>table</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>dorm_amenities</t>
+          <t>sports</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>asdfdsfad</t>
+          <t>table tenis table</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>h17</t>
+          <t>SSO office</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Dorji</t>
+          <t>Mph</t>
         </is>
       </c>
       <c r="G4" s="1" t="n">
-        <v>45282</v>
+        <v>45018</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
+          <t>5642411</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>dsfdsa</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>sports</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>adsf</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>sdfs</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>dfds</t>
+        </is>
+      </c>
+      <c r="G5" s="1" t="n">
+        <v>44898</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>443242</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>scoreboard</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>dorm_amenities</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>basketball scoreboard</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>SSO office</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>SSO</t>
+        </is>
+      </c>
+      <c r="G6" s="1" t="n">
+        <v>44933</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>43542365</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>scoreboard</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>sports</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>basketball scoreboard</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>SSO office</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>SSO</t>
+        </is>
+      </c>
+      <c r="G7" s="1" t="n">
+        <v>44948</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2568742</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Table</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>dorm_amenities</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>study table</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>h17</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>dorji</t>
+        </is>
+      </c>
+      <c r="G8" s="1" t="n">
+        <v>44928</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>254265</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>filter</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>dorm_amenities</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>drinking filter</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>h17</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>sherab</t>
+        </is>
+      </c>
+      <c r="G9" s="1" t="n">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>945829</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>scoreboard</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>dorm_amenities</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>basketball scoreboard</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>SSO office</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>SSO</t>
+        </is>
+      </c>
+      <c r="G10" s="1" t="n">
+        <v>44933</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>5432541</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>filter</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>dorm_amenities</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>drinking filter</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>h17</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>sherab</t>
+        </is>
+      </c>
+      <c r="G11" s="1" t="n">
+        <v>44898</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>1254635u476414526357</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>table</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>sports</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>table tenis table</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>SSO office</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Mph</t>
+        </is>
+      </c>
+      <c r="G12" s="1" t="n">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>134351432</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>filter</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>dorm_amenities</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>drinking filter</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>h17</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>sherab</t>
+        </is>
+      </c>
+      <c r="G13" s="1" t="n">
+        <v>44907</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>123456</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>filter</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>dorm_amenities</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>drinking filter</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>h17</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>sherab</t>
+        </is>
+      </c>
+      <c r="G14" s="1" t="n">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>543542</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>asdf</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>dorm_amenities</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>asdfdsfad</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>adasdf</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>asdf</t>
+        </is>
+      </c>
+      <c r="G15" s="1" t="n">
+        <v>44898</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>t231</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>bed</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>sports</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>table tenis table</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>SSO office</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Mph</t>
+        </is>
+      </c>
+      <c r="G16" s="1" t="n">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>4543</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Table</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>dorm_amenities</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>asdfdsfad</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>h17</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>Dorji</t>
+        </is>
+      </c>
+      <c r="G17" s="1" t="n">
+        <v>44898</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>23452</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>dsfdsa</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>sports</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>adsf</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>sdfs</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>dfds</t>
+        </is>
+      </c>
+      <c r="G18" s="1" t="n">
+        <v>44898</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>1234</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>scoreboard</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>sports</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>basketball scoreboard</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>SSO office</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>SSO</t>
+        </is>
+      </c>
+      <c r="G19" s="1" t="n">
+        <v>44948</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>453543</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>filter</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>dorm_amenities</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>drinking filter</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>h17</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>sherab</t>
+        </is>
+      </c>
+      <c r="G20" s="1" t="n">
+        <v>44907</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>y32431</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>gg</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>IT</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>drinking filter</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>h17</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>sherab</t>
+        </is>
+      </c>
+      <c r="G21" s="1" t="n">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>12345667</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>asdf</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>dorm_amenities</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>asdfdsfad</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>adasdf</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>asdf</t>
+        </is>
+      </c>
+      <c r="G22" s="1" t="n">
+        <v>44898</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>64356365</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Table</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>sports</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>asdfdsfad</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>h17</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>Dorji</t>
+        </is>
+      </c>
+      <c r="G23" s="1" t="n">
+        <v>44978</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>231221</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>dsfdsa</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>sports</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>adsf</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>sdfs</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>dfds</t>
+        </is>
+      </c>
+      <c r="G24" s="1" t="n">
+        <v>44898</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>7657</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>scoreboard</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>sports</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>basketball scoreboard</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>SSO office</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>SSO</t>
+        </is>
+      </c>
+      <c r="G25" s="1" t="n">
+        <v>44948</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>56543</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>filter</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>dorm_amenities</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>drinking filter</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>h17</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>sherab</t>
+        </is>
+      </c>
+      <c r="G26" s="1" t="n">
+        <v>44898</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>45432</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>filter</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>dorm_amenities</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>drinking filter</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>h17</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>sherab</t>
+        </is>
+      </c>
+      <c r="G27" s="1" t="n">
+        <v>44898</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>654365</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>asdf</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>dorm_amenities</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>asdfdsfad</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>adasdf</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>asdf</t>
+        </is>
+      </c>
+      <c r="G28" s="1" t="n">
+        <v>44898</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>65437556</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Table</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>dorm_amenities</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>asdfdsfad</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>h17</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>Dorji</t>
+        </is>
+      </c>
+      <c r="G29" s="1" t="n">
+        <v>44898</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>2131412</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>dsfdsa</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>sports</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>adsf</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>sdfs</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>dfds</t>
+        </is>
+      </c>
+      <c r="G30" s="1" t="n">
+        <v>44898</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>322432</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>scoreboard</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>sports</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>basketball scoreboard</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>SSO office</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>SSO</t>
+        </is>
+      </c>
+      <c r="G31" s="1" t="n">
+        <v>44948</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>98767890</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>filter</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>dorm_amenities</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>drinking filter</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>h17</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>sherab</t>
+        </is>
+      </c>
+      <c r="G32" s="1" t="n">
+        <v>44898</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>2315213</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Table</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>dorm_amenities</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>asdfdsfad</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>h17</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>Dorji</t>
+        </is>
+      </c>
+      <c r="G33" s="1" t="n">
+        <v>44898</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>634577</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>dsfdsa</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>sports</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>adsf</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>sdfs</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>dfds</t>
+        </is>
+      </c>
+      <c r="G34" s="1" t="n">
+        <v>44898</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>653452</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>scoreboard</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>sports</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>basketball scoreboard</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>SSO office</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>SSO</t>
+        </is>
+      </c>
+      <c r="G35" s="1" t="n">
+        <v>44948</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>52454312</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>filter</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>dorm_amenities</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>drinking filter</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>h17</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>sherab</t>
+        </is>
+      </c>
+      <c r="G36" s="1" t="n">
+        <v>44898</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>414562</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>asdf</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>dorm_amenities</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>asdfdsfad</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>adasdf</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>asdf</t>
+        </is>
+      </c>
+      <c r="G37" s="1" t="n">
+        <v>44898</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>451</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Table</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>dorm_amenities</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>asdfdsfad</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>h17</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>Dorji</t>
+        </is>
+      </c>
+      <c r="G38" s="1" t="n">
+        <v>44898</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>556789</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>dsfdsa</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>sports</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>adsf</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>sdfs</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>dfds</t>
+        </is>
+      </c>
+      <c r="G39" s="1" t="n">
+        <v>44898</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>764567</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Table</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>sports</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>asdfdsfad</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>h17</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>Dorji</t>
+        </is>
+      </c>
+      <c r="G40" s="1" t="n">
+        <v>44978</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>1234567</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Table</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>sports</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>asdfdsfad</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>h17</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>Dorji</t>
+        </is>
+      </c>
+      <c r="G41" s="1" t="n">
+        <v>44978</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>347890</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>scoreboard</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>dorm_amenities</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>basketball scoreboard</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>SSO office</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>SSO</t>
+        </is>
+      </c>
+      <c r="G42" s="1" t="n">
+        <v>44933</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>1325442653413440</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Chair</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>dorm_amenities</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>Study chair</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>h17</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>Pema</t>
+        </is>
+      </c>
+      <c r="G43" s="1" t="n">
+        <v>45263</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
           <t>7890</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="B44" t="inlineStr">
         <is>
           <t>Chair</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>dorm_amenities</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>dorm_amenities</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
         <is>
           <t>Study chair</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>h17</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>h17</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
         <is>
           <t>Pema</t>
         </is>
       </c>
-      <c r="G5" s="1" t="n">
+      <c r="G44" s="1" t="n">
         <v>45263</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>674552</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Chair</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>dorm_amenities</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>Study chair</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>h17</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>Pema</t>
+        </is>
+      </c>
+      <c r="G45" s="1" t="n">
+        <v>45263</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Table</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>dorm_amenities</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>study table</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>h17</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>dorji</t>
+        </is>
+      </c>
+      <c r="G46" s="1" t="n">
+        <v>44928</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>34732890</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>table</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>sports</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>table tenis table</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>SSO office</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>Mph</t>
+        </is>
+      </c>
+      <c r="G47" s="1" t="n">
+        <v>45018</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
staff user previlage update
</commit_message>
<xml_diff>
--- a/assets.xlsx
+++ b/assets.xlsx
@@ -416,7 +416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -464,12 +464,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>12345</t>
+          <t>IT657349</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>bed</t>
+          <t>Table</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -479,56 +479,56 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Type_C</t>
+          <t>study table</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Block_C</t>
+          <t>h17</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>pem</t>
+          <t>12190029</t>
         </is>
       </c>
       <c r="G2" s="1" t="n">
-        <v>45068</v>
+        <v>45078</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>A1234567</t>
+          <t>12345</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Projector</t>
+          <t>Chair</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>electronics</t>
+          <t>dorm_amenities</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>EpsonA</t>
+          <t>study chair</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Classroom4</t>
+          <t>H12</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Bsc Cs 3rd year</t>
+          <t>12190023</t>
         </is>
       </c>
       <c r="G3" s="1" t="n">
-        <v>45050</v>
+        <v>45070</v>
       </c>
     </row>
     <row r="4">
@@ -563,18 +563,18 @@
         </is>
       </c>
       <c r="G4" s="1" t="n">
-        <v>45283</v>
+        <v>45074</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>IT657346</t>
+          <t>IT657350</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>table</t>
+          <t>scoreboard</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -584,32 +584,32 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>study table</t>
+          <t>basketball scoreboard</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>h17</t>
+          <t>SSO office</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>12190023</t>
+          <t>12190026</t>
         </is>
       </c>
       <c r="G5" s="1" t="n">
-        <v>44981</v>
+        <v>45079</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>IT657347</t>
+          <t>IT657346</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>chair</t>
+          <t>table</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -619,32 +619,32 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>study chair</t>
+          <t>study table</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>h18</t>
+          <t>h17</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>12190024</t>
+          <t>12190023</t>
         </is>
       </c>
       <c r="G6" s="1" t="n">
-        <v>45010</v>
+        <v>45075</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>IT657348</t>
+          <t>IT657347</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Chair</t>
+          <t>chair</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -654,32 +654,32 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Study chair</t>
+          <t>study chair</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>h17</t>
+          <t>h18</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>12190025</t>
+          <t>12190024</t>
         </is>
       </c>
       <c r="G7" s="1" t="n">
-        <v>45286</v>
+        <v>45076</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>IT657349</t>
+          <t>IT657351</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Table</t>
+          <t>filter</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -689,7 +689,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>study table</t>
+          <t>drinking filter</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -699,22 +699,22 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>12190029</t>
+          <t>12190040</t>
         </is>
       </c>
       <c r="G8" s="1" t="n">
-        <v>45196</v>
+        <v>45080</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>IT657350</t>
+          <t>IT657348</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>scoreboard</t>
+          <t>Chair</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -724,56 +724,21 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>basketball scoreboard</t>
+          <t>Study chair</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>SSO office</t>
+          <t>h17</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>12190026</t>
+          <t>12190025</t>
         </is>
       </c>
       <c r="G9" s="1" t="n">
-        <v>45289</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>IT657351</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>filter</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>dorm_amenities</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>drinking filter</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>h17</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>12190040</t>
-        </is>
-      </c>
-      <c r="G10" s="1" t="n">
-        <v>45290</v>
+        <v>45077</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update on new feature inactive asset and report log
</commit_message>
<xml_diff>
--- a/assets.xlsx
+++ b/assets.xlsx
@@ -416,7 +416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -459,12 +459,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>IT657349</t>
+          <t>IT653459</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Table</t>
+          <t>Chair</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -479,22 +479,22 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>12190029</t>
+          <t>12190025</t>
         </is>
       </c>
       <c r="F2" s="1" t="n">
-        <v>45078</v>
+        <v>45077</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>12345</t>
+          <t>IT653460</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Chair</t>
+          <t>Table</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -504,22 +504,22 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>H12</t>
+          <t>h17</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>12190023</t>
+          <t>12190029</t>
         </is>
       </c>
       <c r="F3" s="1" t="n">
-        <v>45070</v>
+        <v>45078</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>IT657345</t>
+          <t>IT653461</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -539,22 +539,22 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>SSO</t>
+          <t>12190026</t>
         </is>
       </c>
       <c r="F4" s="1" t="n">
-        <v>45074</v>
+        <v>45079</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>IT657350</t>
+          <t>IT653462</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>scoreboard</t>
+          <t>filter</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -564,22 +564,22 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>SSO office</t>
+          <t>h17</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>12190026</t>
+          <t>12190040</t>
         </is>
       </c>
       <c r="F5" s="1" t="n">
-        <v>45079</v>
+        <v>45080</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>IT657346</t>
+          <t>IT65329324</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -594,7 +594,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>h17</t>
+          <t>SSO office</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -603,18 +603,18 @@
         </is>
       </c>
       <c r="F6" s="1" t="n">
-        <v>45075</v>
+        <v>45074</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>IT657347</t>
+          <t>IT65329325</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>chair</t>
+          <t>table</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -624,27 +624,27 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>h18</t>
+          <t>h17</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>12190024</t>
+          <t>12190023</t>
         </is>
       </c>
       <c r="F7" s="1" t="n">
-        <v>45076</v>
+        <v>45075</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>IT657351</t>
+          <t>IT65329326</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>filter</t>
+          <t>chair</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -654,22 +654,22 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>h17</t>
+          <t>h18</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>12190040</t>
+          <t>12190024</t>
         </is>
       </c>
       <c r="F8" s="1" t="n">
-        <v>45080</v>
+        <v>45076</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>IT657348</t>
+          <t>IT65329327</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -694,6 +694,306 @@
       </c>
       <c r="F9" s="1" t="n">
         <v>45077</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>IT657348</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Chair</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>dorm_amenities</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>h17</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>12190025</t>
+        </is>
+      </c>
+      <c r="F10" s="1" t="n">
+        <v>45077</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>IT657347</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>chair</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>dorm_amenities</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Y18</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>12190024</t>
+        </is>
+      </c>
+      <c r="F11" s="1" t="n">
+        <v>45076</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>IT657346</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>table</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>dorm_amenities</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>h17</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>12190023</t>
+        </is>
+      </c>
+      <c r="F12" s="1" t="n">
+        <v>45075</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>IT65329328</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Table</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>dorm_amenities</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>h17</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>12190029</t>
+        </is>
+      </c>
+      <c r="F13" s="1" t="n">
+        <v>45078</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>IT657349</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Table</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>dorm_amenities</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>h17</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>12190029</t>
+        </is>
+      </c>
+      <c r="F14" s="1" t="n">
+        <v>45078</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>IT657350</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>scoreboard</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>dorm_amenities</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>SSO office</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>12190026</t>
+        </is>
+      </c>
+      <c r="F15" s="1" t="n">
+        <v>45079</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>IT65329329</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>scoreboard</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>dorm_amenities</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>SSO office</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>12190026</t>
+        </is>
+      </c>
+      <c r="F16" s="1" t="n">
+        <v>45079</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>IT657345</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Bed type A</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>dorm_amenities</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>SSO office</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>12190023</t>
+        </is>
+      </c>
+      <c r="F17" s="1" t="n">
+        <v>45074</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>IT653456</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>table</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>dorm_amenities</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>SSO office</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>12190023</t>
+        </is>
+      </c>
+      <c r="F18" s="1" t="n">
+        <v>45074</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>IT653457</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>table</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>dorm_amenities</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>h17</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>12190023</t>
+        </is>
+      </c>
+      <c r="F19" s="1" t="n">
+        <v>45075</v>
       </c>
     </row>
   </sheetData>

</xml_diff>